<commit_message>
Create Fgraph.m and edit Book2.xlsx
</commit_message>
<xml_diff>
--- a/Metodos numercios/Book2.xlsx
+++ b/Metodos numercios/Book2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f04136d1dafd546/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f04136d1dafd546/Desktop/NRCMetodosNumericos/GeneralScriptMatlab/Metodos numercios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B0CD552-EAAD-44C6-A999-9EF48E4E40CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{6B0CD552-EAAD-44C6-A999-9EF48E4E40CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79A85A79-1431-4400-9693-DBD833FB1890}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5D12A085-D023-4C6C-A8B2-65EA175A4E79}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -69,13 +69,13 @@
     <t>xy</t>
   </si>
   <si>
-    <t>x^2</t>
+    <t>xcua</t>
   </si>
   <si>
-    <t>y^2</t>
+    <t>ycua</t>
   </si>
   <si>
-    <t>(xy)^2</t>
+    <t>xycua</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>